<commit_message>
prototype a few verification terms
</commit_message>
<xml_diff>
--- a/Remo.Test/Artifacts/TEST_TEMPLATE.xlsx
+++ b/Remo.Test/Artifacts/TEST_TEMPLATE.xlsx
@@ -12,10 +12,12 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="14625" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCase-1" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCase-2" sheetId="5" r:id="rId2"/>
-    <sheet name="Batch-Template" sheetId="4" r:id="rId3"/>
-    <sheet name="List" sheetId="3" r:id="rId4"/>
+    <sheet name="Select" sheetId="7" r:id="rId1"/>
+    <sheet name="Text" sheetId="10" r:id="rId2"/>
+    <sheet name="TestCase-1" sheetId="1" r:id="rId3"/>
+    <sheet name="TestCase-2" sheetId="5" r:id="rId4"/>
+    <sheet name="Batch-Template" sheetId="4" r:id="rId5"/>
+    <sheet name="List" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Actions">List!$A$1:$A$9</definedName>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="64">
   <si>
     <t>Action</t>
   </si>
@@ -164,13 +166,67 @@
   </si>
   <si>
     <t>Log In</t>
+  </si>
+  <si>
+    <t>http://joljet.net/stub.html</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>id = city</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Equals</t>
+  </si>
+  <si>
+    <t>Assertion</t>
+  </si>
+  <si>
+    <t>Contains</t>
+  </si>
+  <si>
+    <t>Exists</t>
+  </si>
+  <si>
+    <t>id = textfield</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>City Name = Melbourne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +288,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,8 +320,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -517,12 +585,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -602,6 +743,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -913,6 +1067,738 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="55.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A26:A30"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30">
+      <formula1>Actions</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F30">
+      <formula1>Result</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="55.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="30"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="30"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="30"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A26:A30"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F30">
+      <formula1>Result</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30">
+      <formula1>Actions</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E5" sqref="B2:E5"/>
     </sheetView>
   </sheetViews>
@@ -1285,14 +2171,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1649,7 +2535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1663,21 +2549,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1687,8 +2577,20 @@
       <c r="H1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K1" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1698,53 +2600,163 @@
       <c r="H2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="39"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="40"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="41"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4" s="40"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="41"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5" s="40"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="41"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6" s="40"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="41"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7" s="40"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8" s="40"/>
+      <c r="L8" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="40"/>
+      <c r="N8" s="41"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
+      <c r="K9" s="40"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K10" s="40"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K11" s="40"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="41"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K12" s="40"/>
+      <c r="L12" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="40"/>
+      <c r="N12" s="41"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K13" s="40"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K14" s="40"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K15" s="40"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="41"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K16" s="40"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="41"/>
+    </row>
+    <row r="17" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K17" s="40"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="41"/>
+    </row>
+    <row r="18" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K18" s="40"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="41"/>
+    </row>
+    <row r="19" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K19" s="40"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="41"/>
     </row>
   </sheetData>
   <sortState ref="A1:B8">

</xml_diff>

<commit_message>
add delay before taking screenshot
Some page just dodgy
</commit_message>
<xml_diff>
--- a/Remo.Test/Artifacts/TEST_TEMPLATE.xlsx
+++ b/Remo.Test/Artifacts/TEST_TEMPLATE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="14625" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="14625" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Select" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
   <si>
     <t>Action</t>
   </si>
@@ -233,6 +233,33 @@
   </si>
   <si>
     <t>login-page.png</t>
+  </si>
+  <si>
+    <t>https://github.com/</t>
+  </si>
+  <si>
+    <t>Pick a username</t>
+  </si>
+  <si>
+    <t>username1</t>
+  </si>
+  <si>
+    <t>name = user[login]</t>
+  </si>
+  <si>
+    <t>name = user[email]</t>
+  </si>
+  <si>
+    <t>You email</t>
+  </si>
+  <si>
+    <t>email1@foo.bar</t>
+  </si>
+  <si>
+    <t>name = user[password]</t>
+  </si>
+  <si>
+    <t>signup-github.png</t>
   </si>
 </sst>
 </file>
@@ -707,7 +734,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -786,6 +813,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="22" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -810,6 +840,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1275,7 +1306,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -1284,7 +1315,7 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
@@ -1293,7 +1324,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
@@ -1302,7 +1333,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -1311,7 +1342,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -1320,7 +1351,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -1329,7 +1360,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -1349,7 +1380,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1358,7 +1389,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1367,7 +1398,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1376,7 +1407,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -1385,7 +1416,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -1394,7 +1425,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -1414,7 +1445,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -1423,7 +1454,7 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -1432,7 +1463,7 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -1441,7 +1472,7 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -1450,7 +1481,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="14"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
@@ -1644,7 +1675,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -1653,7 +1684,7 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
@@ -1662,7 +1693,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
@@ -1671,7 +1702,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -1680,7 +1711,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -1689,7 +1720,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -1698,7 +1729,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -1718,7 +1749,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1727,7 +1758,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1736,7 +1767,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1745,7 +1776,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -1754,7 +1785,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -1763,7 +1794,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -1783,7 +1814,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -1792,7 +1823,7 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -1801,7 +1832,7 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -1810,7 +1841,7 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -1819,7 +1850,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="14"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
@@ -1853,8 +1884,8 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,7 +2044,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -2022,7 +2053,7 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
@@ -2031,7 +2062,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
@@ -2040,7 +2071,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -2049,7 +2080,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -2058,7 +2089,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -2067,7 +2098,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -2087,7 +2118,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -2096,7 +2127,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -2105,7 +2136,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -2114,7 +2145,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -2123,7 +2154,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -2132,7 +2163,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -2152,7 +2183,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -2161,7 +2192,7 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -2170,7 +2201,7 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -2179,7 +2210,7 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -2188,7 +2219,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="14"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
@@ -2373,7 +2404,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="13"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -2382,7 +2413,7 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
@@ -2391,7 +2422,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
@@ -2400,7 +2431,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -2409,7 +2440,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -2418,7 +2449,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -2427,7 +2458,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -2447,7 +2478,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -2456,7 +2487,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -2465,7 +2496,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -2474,7 +2505,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -2483,7 +2514,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -2492,7 +2523,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -2512,7 +2543,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -2521,7 +2552,7 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -2530,7 +2561,7 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -2539,7 +2570,7 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -2548,7 +2579,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="14"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
@@ -2585,8 +2616,8 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2594,7 +2625,7 @@
     <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" customWidth="1"/>
     <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="55.140625" customWidth="1"/>
@@ -2712,28 +2743,49 @@
       <c r="A7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
+      <c r="B7" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>68</v>
+      </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
+      <c r="B8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>71</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
+      <c r="B9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
     </row>
@@ -2741,24 +2793,36 @@
       <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
+      <c r="B10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="6">
+        <v>121212</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26" t="s">
+        <v>76</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="13"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
@@ -2767,7 +2831,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="13"/>
       <c r="C13" s="5"/>
       <c r="D13" s="6"/>
@@ -2776,7 +2840,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -2785,7 +2849,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -2794,7 +2858,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="13"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
@@ -2803,7 +2867,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="13"/>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -2823,7 +2887,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="13"/>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -2832,7 +2896,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="13"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -2841,7 +2905,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="13"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -2850,7 +2914,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="13"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -2859,7 +2923,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="13"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -2868,7 +2932,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="13"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
@@ -2888,7 +2952,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="13"/>
       <c r="C26" s="5"/>
       <c r="D26" s="6"/>
@@ -2897,7 +2961,7 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="13"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
@@ -2906,7 +2970,7 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="13"/>
       <c r="C28" s="5"/>
       <c r="D28" s="6"/>
@@ -2915,7 +2979,7 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="13"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -2924,7 +2988,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="49"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="14"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
@@ -2948,9 +3012,10 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2996,10 +3061,10 @@
       <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="50"/>
+      <c r="M1" s="51"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -3148,12 +3213,12 @@
       <c r="N14" s="35"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K16" s="34" t="s">

</xml_diff>